<commit_message>
auto commit @16.12.2020: 21:31:21,37
</commit_message>
<xml_diff>
--- a/Kommentare ICS und Testfälle.xlsx
+++ b/Kommentare ICS und Testfälle.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Benutzer\Henry\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Benutzer\Henry\Downloads\Abschlussarbeit_H-BRS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA0E630-87FB-4DCC-9452-A813D50211C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC79CFB4-5760-44A2-A65A-3AA3A0AAF82E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Test Documentation'!$B$1:$B$474</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Test Documentation'!$A$1:$O$117</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -82,30 +82,6 @@
           <t xml:space="preserve">
 Warum werden unterschiedliche Versionen verwendet?
 </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G28" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Aden, Adil:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Würde dieser Punkt vergessen oder ist die Umsetzung schwer?</t>
         </r>
       </text>
     </comment>
@@ -234,7 +210,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1436" uniqueCount="648">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1437" uniqueCount="648">
   <si>
     <t>Im Rahmen von [BSI TR-03148 -P] muss ein Implementation Conformance Statement ausgefüllt werden. Im folgenden finden Sie eine Vorlage für das ICS. Das Originaldokument ist auf Englisch, weswegen hier die englischen Formulierungen übernommen wurden, da keine offizielle Übersetzung des Dokuments existiert. Die Eintragungen können aber auf deutsch oder englisch gemacht werden. Die hier eingetragenen Beispieldaten sind durch Echtdaten zu ersetzen. Alternativ oder ergänzend zu dem ICS in dieser Tabelle kann auch das ICS aus [BSI TR-03148-P] als Vorlage genutzt werden.</t>
   </si>
@@ -6302,104 +6278,104 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="4" borderId="22" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="41" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="4" borderId="35" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="41" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -6808,19 +6784,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="218" t="s">
+      <c r="A2" s="205" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="218"/>
-      <c r="C2" s="218"/>
-      <c r="D2" s="218"/>
-      <c r="E2" s="218"/>
-      <c r="F2" s="218"/>
-      <c r="G2" s="218"/>
-      <c r="H2" s="218"/>
-      <c r="I2" s="218"/>
-      <c r="J2" s="218"/>
-      <c r="K2" s="218"/>
+      <c r="B2" s="205"/>
+      <c r="C2" s="205"/>
+      <c r="D2" s="205"/>
+      <c r="E2" s="205"/>
+      <c r="F2" s="205"/>
+      <c r="G2" s="205"/>
+      <c r="H2" s="205"/>
+      <c r="I2" s="205"/>
+      <c r="J2" s="205"/>
+      <c r="K2" s="205"/>
     </row>
     <row r="4" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6829,10 +6805,10 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="229" t="s">
+      <c r="A6" s="206" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="229"/>
+      <c r="B6" s="206"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -6847,38 +6823,38 @@
       <c r="A7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="230" t="s">
+      <c r="B7" s="207" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="230"/>
+      <c r="C7" s="207"/>
       <c r="D7" s="7"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="231" t="s">
+      <c r="B8" s="208" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="231"/>
+      <c r="C8" s="208"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="231" t="s">
+      <c r="B9" s="208" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="231"/>
+      <c r="C9" s="208"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="226" t="s">
+      <c r="B10" s="209" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="226"/>
+      <c r="C10" s="209"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="8"/>
@@ -6890,86 +6866,86 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="227" t="s">
+      <c r="A14" s="210" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="227"/>
+      <c r="B14" s="210"/>
     </row>
     <row r="15" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="228" t="s">
+      <c r="B15" s="211" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="228"/>
-      <c r="D15" s="228"/>
+      <c r="C15" s="211"/>
+      <c r="D15" s="211"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="221" t="s">
+      <c r="B16" s="212" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="221"/>
-      <c r="D16" s="221"/>
+      <c r="C16" s="212"/>
+      <c r="D16" s="212"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="223" t="s">
+      <c r="B17" s="213" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="223"/>
-      <c r="D17" s="223"/>
-      <c r="E17" s="223"/>
-      <c r="F17" s="223"/>
-      <c r="G17" s="223"/>
-      <c r="H17" s="223"/>
+      <c r="C17" s="213"/>
+      <c r="D17" s="213"/>
+      <c r="E17" s="213"/>
+      <c r="F17" s="213"/>
+      <c r="G17" s="213"/>
+      <c r="H17" s="213"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="223" t="s">
+      <c r="B18" s="213" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="223"/>
-      <c r="D18" s="223"/>
-      <c r="E18" s="223"/>
-      <c r="F18" s="223"/>
-      <c r="G18" s="223"/>
-      <c r="H18" s="223"/>
+      <c r="C18" s="213"/>
+      <c r="D18" s="213"/>
+      <c r="E18" s="213"/>
+      <c r="F18" s="213"/>
+      <c r="G18" s="213"/>
+      <c r="H18" s="213"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="221" t="s">
+      <c r="B19" s="212" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="221"/>
-      <c r="D19" s="221"/>
+      <c r="C19" s="212"/>
+      <c r="D19" s="212"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="224" t="s">
+      <c r="B20" s="214" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="224"/>
-      <c r="D20" s="224"/>
+      <c r="C20" s="214"/>
+      <c r="D20" s="214"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="221"/>
-      <c r="C21" s="221"/>
-      <c r="D21" s="221"/>
+      <c r="B21" s="212"/>
+      <c r="C21" s="212"/>
+      <c r="D21" s="212"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
@@ -6977,70 +6953,70 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="225" t="s">
+      <c r="A25" s="215" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="225"/>
+      <c r="B25" s="215"/>
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="222" t="s">
+      <c r="B26" s="216" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="222"/>
-      <c r="D26" s="222"/>
+      <c r="C26" s="216"/>
+      <c r="D26" s="216"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="221" t="s">
+      <c r="B27" s="212" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="221"/>
-      <c r="D27" s="221"/>
+      <c r="C27" s="212"/>
+      <c r="D27" s="212"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="221" t="s">
+      <c r="B28" s="212" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="221"/>
-      <c r="D28" s="221"/>
+      <c r="C28" s="212"/>
+      <c r="D28" s="212"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="221" t="s">
+      <c r="B29" s="212" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="221"/>
-      <c r="D29" s="221"/>
+      <c r="C29" s="212"/>
+      <c r="D29" s="212"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="221" t="s">
+      <c r="B30" s="212" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="221"/>
-      <c r="D30" s="221"/>
+      <c r="C30" s="212"/>
+      <c r="D30" s="212"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="221" t="s">
+      <c r="B31" s="212" t="s">
         <v>36</v>
       </c>
-      <c r="C31" s="221"/>
-      <c r="D31" s="221"/>
+      <c r="C31" s="212"/>
+      <c r="D31" s="212"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="16"/>
@@ -7052,13 +7028,13 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="218" t="s">
+      <c r="A34" s="205" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="218"/>
-      <c r="C34" s="218"/>
-      <c r="D34" s="218"/>
-      <c r="E34" s="218"/>
+      <c r="B34" s="205"/>
+      <c r="C34" s="205"/>
+      <c r="D34" s="205"/>
+      <c r="E34" s="205"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
@@ -7414,13 +7390,13 @@
       </c>
     </row>
     <row r="58" spans="1:11" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="218" t="s">
+      <c r="A58" s="205" t="s">
         <v>63</v>
       </c>
-      <c r="B58" s="218"/>
-      <c r="C58" s="218"/>
-      <c r="D58" s="218"/>
-      <c r="E58" s="218"/>
+      <c r="B58" s="205"/>
+      <c r="C58" s="205"/>
+      <c r="D58" s="205"/>
+      <c r="E58" s="205"/>
     </row>
     <row r="59" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="60" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7531,13 +7507,13 @@
       </c>
     </row>
     <row r="69" spans="1:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="218" t="s">
+      <c r="A69" s="205" t="s">
         <v>69</v>
       </c>
-      <c r="B69" s="218"/>
-      <c r="C69" s="218"/>
-      <c r="D69" s="218"/>
-      <c r="E69" s="218"/>
+      <c r="B69" s="205"/>
+      <c r="C69" s="205"/>
+      <c r="D69" s="205"/>
+      <c r="E69" s="205"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="26"/>
@@ -7560,12 +7536,12 @@
       </c>
     </row>
     <row r="74" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="218" t="s">
+      <c r="A74" s="205" t="s">
         <v>74</v>
       </c>
-      <c r="B74" s="218"/>
-      <c r="C74" s="218"/>
-      <c r="D74" s="218"/>
+      <c r="B74" s="205"/>
+      <c r="C74" s="205"/>
+      <c r="D74" s="205"/>
       <c r="E74" s="27"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -7577,12 +7553,12 @@
       </c>
     </row>
     <row r="79" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="218" t="s">
+      <c r="A79" s="205" t="s">
         <v>76</v>
       </c>
-      <c r="B79" s="218"/>
-      <c r="C79" s="218"/>
-      <c r="D79" s="218"/>
+      <c r="B79" s="205"/>
+      <c r="C79" s="205"/>
+      <c r="D79" s="205"/>
     </row>
     <row r="81" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="28" t="s">
@@ -7662,13 +7638,13 @@
       </c>
     </row>
     <row r="90" spans="1:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="219" t="s">
+      <c r="A90" s="217" t="s">
         <v>561</v>
       </c>
-      <c r="B90" s="219"/>
-      <c r="C90" s="219"/>
-      <c r="D90" s="219"/>
-      <c r="E90" s="219"/>
+      <c r="B90" s="217"/>
+      <c r="C90" s="217"/>
+      <c r="D90" s="217"/>
+      <c r="E90" s="217"/>
     </row>
     <row r="92" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="20" t="s">
@@ -7769,10 +7745,10 @@
       </c>
     </row>
     <row r="101" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="220" t="s">
+      <c r="A101" s="218" t="s">
         <v>93</v>
       </c>
-      <c r="B101" s="220"/>
+      <c r="B101" s="218"/>
     </row>
     <row r="103" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
@@ -7788,12 +7764,12 @@
       </c>
     </row>
     <row r="107" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="219" t="s">
+      <c r="A107" s="217" t="s">
         <v>562</v>
       </c>
-      <c r="B107" s="219"/>
-      <c r="C107" s="219"/>
-      <c r="D107" s="219"/>
+      <c r="B107" s="217"/>
+      <c r="C107" s="217"/>
+      <c r="D107" s="217"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
@@ -7901,12 +7877,12 @@
       <c r="B116" s="33"/>
     </row>
     <row r="119" spans="1:4" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="214" t="s">
+      <c r="A119" s="219" t="s">
         <v>101</v>
       </c>
-      <c r="B119" s="214"/>
-      <c r="C119" s="214"/>
-      <c r="D119" s="214"/>
+      <c r="B119" s="219"/>
+      <c r="C119" s="219"/>
+      <c r="D119" s="219"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="10" t="s">
@@ -7959,9 +7935,9 @@
       <c r="D126" s="22"/>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="217"/>
-      <c r="B127" s="217"/>
-      <c r="C127" s="217"/>
+      <c r="A127" s="220"/>
+      <c r="B127" s="220"/>
+      <c r="C127" s="220"/>
     </row>
     <row r="129" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A129" s="35" t="s">
@@ -7969,12 +7945,12 @@
       </c>
     </row>
     <row r="130" spans="1:4" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="210" t="s">
+      <c r="A130" s="221" t="s">
         <v>103</v>
       </c>
-      <c r="B130" s="210"/>
-      <c r="C130" s="210"/>
-      <c r="D130" s="210"/>
+      <c r="B130" s="221"/>
+      <c r="C130" s="221"/>
+      <c r="D130" s="221"/>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="10" t="s">
@@ -8092,12 +8068,12 @@
       </c>
     </row>
     <row r="143" spans="1:4" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="210" t="s">
+      <c r="A143" s="221" t="s">
         <v>121</v>
       </c>
-      <c r="B143" s="210"/>
-      <c r="C143" s="210"/>
-      <c r="D143" s="210"/>
+      <c r="B143" s="221"/>
+      <c r="C143" s="221"/>
+      <c r="D143" s="221"/>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="10" t="s">
@@ -8142,18 +8118,18 @@
       <c r="C147" s="37"/>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="207" t="s">
+      <c r="A148" s="222" t="s">
         <v>129</v>
       </c>
-      <c r="B148" s="207"/>
+      <c r="B148" s="222"/>
     </row>
     <row r="150" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="210" t="s">
+      <c r="A150" s="221" t="s">
         <v>130</v>
       </c>
-      <c r="B150" s="210"/>
-      <c r="C150" s="210"/>
-      <c r="D150" s="210"/>
+      <c r="B150" s="221"/>
+      <c r="C150" s="221"/>
+      <c r="D150" s="221"/>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="10" t="s">
@@ -8184,12 +8160,12 @@
       <c r="B155" s="25"/>
     </row>
     <row r="157" spans="1:4" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="214" t="s">
+      <c r="A157" s="219" t="s">
         <v>132</v>
       </c>
-      <c r="B157" s="214"/>
-      <c r="C157" s="214"/>
-      <c r="D157" s="214"/>
+      <c r="B157" s="219"/>
+      <c r="C157" s="219"/>
+      <c r="D157" s="219"/>
     </row>
     <row r="158" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A158" s="10" t="s">
@@ -8255,10 +8231,10 @@
       <c r="A164" s="38"/>
     </row>
     <row r="165" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="206" t="s">
+      <c r="A165" s="223" t="s">
         <v>136</v>
       </c>
-      <c r="B165" s="206"/>
+      <c r="B165" s="223"/>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="10" t="s">
@@ -8293,36 +8269,36 @@
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" s="207" t="s">
+      <c r="A170" s="222" t="s">
         <v>142</v>
       </c>
-      <c r="B170" s="207"/>
+      <c r="B170" s="222"/>
     </row>
     <row r="172" spans="1:4" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="210" t="s">
+      <c r="A172" s="221" t="s">
         <v>143</v>
       </c>
-      <c r="B172" s="210"/>
-      <c r="C172" s="210"/>
-      <c r="D172" s="210"/>
+      <c r="B172" s="221"/>
+      <c r="C172" s="221"/>
+      <c r="D172" s="221"/>
     </row>
     <row r="173" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="39" t="s">
         <v>144</v>
       </c>
-      <c r="B173" s="216" t="s">
+      <c r="B173" s="224" t="s">
         <v>145</v>
       </c>
-      <c r="C173" s="216"/>
-      <c r="D173" s="216"/>
+      <c r="C173" s="224"/>
+      <c r="D173" s="224"/>
     </row>
     <row r="175" spans="1:4" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A175" s="213" t="s">
+      <c r="A175" s="225" t="s">
         <v>146</v>
       </c>
-      <c r="B175" s="213"/>
-      <c r="C175" s="213"/>
-      <c r="D175" s="213"/>
+      <c r="B175" s="225"/>
+      <c r="C175" s="225"/>
+      <c r="D175" s="225"/>
     </row>
     <row r="177" spans="1:7" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A177" s="40" t="s">
@@ -8371,20 +8347,20 @@
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A181" s="207"/>
-      <c r="B181" s="207"/>
+      <c r="A181" s="222"/>
+      <c r="B181" s="222"/>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="42"/>
       <c r="B182" s="42"/>
     </row>
     <row r="183" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A183" s="214" t="s">
+      <c r="A183" s="219" t="s">
         <v>564</v>
       </c>
-      <c r="B183" s="214"/>
-      <c r="C183" s="214"/>
-      <c r="D183" s="214"/>
+      <c r="B183" s="219"/>
+      <c r="C183" s="219"/>
+      <c r="D183" s="219"/>
     </row>
     <row r="184" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="10" t="s">
@@ -8425,20 +8401,20 @@
       <c r="D187" s="22"/>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A188" s="215"/>
-      <c r="B188" s="215"/>
+      <c r="A188" s="226"/>
+      <c r="B188" s="226"/>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" s="43"/>
       <c r="B189" s="43"/>
     </row>
     <row r="190" spans="1:7" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A190" s="210" t="s">
+      <c r="A190" s="221" t="s">
         <v>159</v>
       </c>
-      <c r="B190" s="210"/>
-      <c r="C190" s="210"/>
-      <c r="D190" s="210"/>
+      <c r="B190" s="221"/>
+      <c r="C190" s="221"/>
+      <c r="D190" s="221"/>
       <c r="F190" s="3" t="s">
         <v>160</v>
       </c>
@@ -8477,12 +8453,12 @@
       </c>
     </row>
     <row r="199" spans="1:4" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A199" s="211" t="s">
+      <c r="A199" s="227" t="s">
         <v>164</v>
       </c>
-      <c r="B199" s="211"/>
-      <c r="C199" s="211"/>
-      <c r="D199" s="211"/>
+      <c r="B199" s="227"/>
+      <c r="C199" s="227"/>
+      <c r="D199" s="227"/>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" s="45" t="s">
@@ -8521,20 +8497,20 @@
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A205" s="207"/>
-      <c r="B205" s="207"/>
+      <c r="A205" s="222"/>
+      <c r="B205" s="222"/>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" s="42"/>
       <c r="B206" s="42"/>
     </row>
     <row r="207" spans="1:4" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A207" s="205" t="s">
+      <c r="A207" s="228" t="s">
         <v>170</v>
       </c>
-      <c r="B207" s="205"/>
-      <c r="C207" s="205"/>
-      <c r="D207" s="205"/>
+      <c r="B207" s="228"/>
+      <c r="C207" s="228"/>
+      <c r="D207" s="228"/>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" s="10" t="s">
@@ -8565,19 +8541,19 @@
       <c r="B213" s="22"/>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A214" s="207"/>
-      <c r="B214" s="207"/>
+      <c r="A214" s="222"/>
+      <c r="B214" s="222"/>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" s="47"/>
     </row>
     <row r="216" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A216" s="212" t="s">
+      <c r="A216" s="229" t="s">
         <v>566</v>
       </c>
-      <c r="B216" s="212"/>
-      <c r="C216" s="212"/>
-      <c r="D216" s="212"/>
+      <c r="B216" s="229"/>
+      <c r="C216" s="229"/>
+      <c r="D216" s="229"/>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" s="10" t="s">
@@ -8626,12 +8602,12 @@
       <c r="B222" s="42"/>
     </row>
     <row r="223" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A223" s="210" t="s">
+      <c r="A223" s="221" t="s">
         <v>174</v>
       </c>
-      <c r="B223" s="210"/>
-      <c r="C223" s="210"/>
-      <c r="D223" s="210"/>
+      <c r="B223" s="221"/>
+      <c r="C223" s="221"/>
+      <c r="D223" s="221"/>
     </row>
     <row r="224" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A224" s="48" t="s">
@@ -8642,12 +8618,12 @@
       </c>
     </row>
     <row r="226" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A226" s="205" t="s">
+      <c r="A226" s="228" t="s">
         <v>177</v>
       </c>
-      <c r="B226" s="205"/>
-      <c r="C226" s="205"/>
-      <c r="D226" s="205"/>
+      <c r="B226" s="228"/>
+      <c r="C226" s="228"/>
+      <c r="D226" s="228"/>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" s="48" t="s">
@@ -8663,12 +8639,12 @@
       </c>
     </row>
     <row r="230" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A230" s="205" t="s">
+      <c r="A230" s="228" t="s">
         <v>180</v>
       </c>
-      <c r="B230" s="205"/>
-      <c r="C230" s="205"/>
-      <c r="D230" s="205"/>
+      <c r="B230" s="228"/>
+      <c r="C230" s="228"/>
+      <c r="D230" s="228"/>
     </row>
     <row r="231" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A231" s="48" t="s">
@@ -8684,12 +8660,12 @@
       </c>
     </row>
     <row r="234" spans="1:5" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A234" s="205" t="s">
+      <c r="A234" s="228" t="s">
         <v>183</v>
       </c>
-      <c r="B234" s="205"/>
-      <c r="C234" s="205"/>
-      <c r="D234" s="205"/>
+      <c r="B234" s="228"/>
+      <c r="C234" s="228"/>
+      <c r="D234" s="228"/>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" s="48" t="s">
@@ -8716,12 +8692,12 @@
       </c>
     </row>
     <row r="239" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A239" s="205" t="s">
+      <c r="A239" s="228" t="s">
         <v>188</v>
       </c>
-      <c r="B239" s="205"/>
-      <c r="C239" s="205"/>
-      <c r="D239" s="205"/>
+      <c r="B239" s="228"/>
+      <c r="C239" s="228"/>
+      <c r="D239" s="228"/>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" s="48" t="s">
@@ -8735,10 +8711,10 @@
       </c>
     </row>
     <row r="241" spans="1:5" ht="144.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D241" s="209" t="s">
+      <c r="D241" s="230" t="s">
         <v>191</v>
       </c>
-      <c r="E241" s="209"/>
+      <c r="E241" s="230"/>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D242" s="3" t="s">
@@ -8754,12 +8730,12 @@
       </c>
     </row>
     <row r="245" spans="1:5" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A245" s="205" t="s">
+      <c r="A245" s="228" t="s">
         <v>195</v>
       </c>
-      <c r="B245" s="205"/>
-      <c r="C245" s="205"/>
-      <c r="D245" s="205"/>
+      <c r="B245" s="228"/>
+      <c r="C245" s="228"/>
+      <c r="D245" s="228"/>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" s="48" t="s">
@@ -8770,12 +8746,12 @@
       </c>
     </row>
     <row r="248" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A248" s="210" t="s">
+      <c r="A248" s="221" t="s">
         <v>197</v>
       </c>
-      <c r="B248" s="210"/>
-      <c r="C248" s="210"/>
-      <c r="D248" s="210"/>
+      <c r="B248" s="221"/>
+      <c r="C248" s="221"/>
+      <c r="D248" s="221"/>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" s="48" t="s">
@@ -8788,12 +8764,12 @@
       </c>
     </row>
     <row r="252" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A252" s="205" t="s">
+      <c r="A252" s="228" t="s">
         <v>199</v>
       </c>
-      <c r="B252" s="205"/>
-      <c r="C252" s="205"/>
-      <c r="D252" s="205"/>
+      <c r="B252" s="228"/>
+      <c r="C252" s="228"/>
+      <c r="D252" s="228"/>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" s="48" t="s">
@@ -8826,12 +8802,12 @@
       </c>
     </row>
     <row r="257" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A257" s="205" t="s">
+      <c r="A257" s="228" t="s">
         <v>204</v>
       </c>
-      <c r="B257" s="205"/>
-      <c r="C257" s="205"/>
-      <c r="D257" s="205"/>
+      <c r="B257" s="228"/>
+      <c r="C257" s="228"/>
+      <c r="D257" s="228"/>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" s="10" t="s">
@@ -8881,11 +8857,11 @@
       <c r="B263" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="C263" s="208" t="s">
+      <c r="C263" s="231" t="s">
         <v>215</v>
       </c>
-      <c r="D263" s="208"/>
-      <c r="E263" s="208"/>
+      <c r="D263" s="231"/>
+      <c r="E263" s="231"/>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" s="42"/>
@@ -8897,10 +8873,10 @@
       </c>
     </row>
     <row r="266" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A266" s="205" t="s">
+      <c r="A266" s="228" t="s">
         <v>217</v>
       </c>
-      <c r="B266" s="205"/>
+      <c r="B266" s="228"/>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" s="49"/>
@@ -8911,12 +8887,12 @@
       </c>
     </row>
     <row r="269" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A269" s="205" t="s">
+      <c r="A269" s="228" t="s">
         <v>219</v>
       </c>
-      <c r="B269" s="205"/>
-      <c r="C269" s="205"/>
-      <c r="D269" s="205"/>
+      <c r="B269" s="228"/>
+      <c r="C269" s="228"/>
+      <c r="D269" s="228"/>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" s="48" t="s">
@@ -8927,12 +8903,12 @@
       </c>
     </row>
     <row r="272" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A272" s="205" t="s">
+      <c r="A272" s="228" t="s">
         <v>221</v>
       </c>
-      <c r="B272" s="205"/>
-      <c r="C272" s="205"/>
-      <c r="D272" s="205"/>
+      <c r="B272" s="228"/>
+      <c r="C272" s="228"/>
+      <c r="D272" s="228"/>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A273" s="48" t="s">
@@ -8944,16 +8920,16 @@
     </row>
     <row r="274" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="275" spans="1:4" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A275" s="205" t="s">
+      <c r="A275" s="228" t="s">
         <v>222</v>
       </c>
-      <c r="B275" s="205"/>
+      <c r="B275" s="228"/>
     </row>
     <row r="276" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A276" s="205" t="s">
+      <c r="A276" s="228" t="s">
         <v>223</v>
       </c>
-      <c r="B276" s="205"/>
+      <c r="B276" s="228"/>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A277" s="48" t="s">
@@ -8964,12 +8940,12 @@
       </c>
     </row>
     <row r="279" spans="1:4" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A279" s="206" t="s">
+      <c r="A279" s="223" t="s">
         <v>569</v>
       </c>
-      <c r="B279" s="206"/>
-      <c r="C279" s="206"/>
-      <c r="D279" s="206"/>
+      <c r="B279" s="223"/>
+      <c r="C279" s="223"/>
+      <c r="D279" s="223"/>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A280" s="10" t="s">
@@ -9002,8 +8978,8 @@
       <c r="D282" s="24"/>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A283" s="207"/>
-      <c r="B283" s="207"/>
+      <c r="A283" s="222"/>
+      <c r="B283" s="222"/>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A284" s="42"/>
@@ -9028,12 +9004,12 @@
       </c>
     </row>
     <row r="289" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A289" s="205" t="s">
+      <c r="A289" s="228" t="s">
         <v>228</v>
       </c>
-      <c r="B289" s="205"/>
-      <c r="C289" s="205"/>
-      <c r="D289" s="205"/>
+      <c r="B289" s="228"/>
+      <c r="C289" s="228"/>
+      <c r="D289" s="228"/>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A290" s="48" t="s">
@@ -9044,12 +9020,12 @@
       </c>
     </row>
     <row r="292" spans="1:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A292" s="206" t="s">
+      <c r="A292" s="223" t="s">
         <v>572</v>
       </c>
-      <c r="B292" s="206"/>
-      <c r="C292" s="206"/>
-      <c r="D292" s="206"/>
+      <c r="B292" s="223"/>
+      <c r="C292" s="223"/>
+      <c r="D292" s="223"/>
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A294" s="52" t="s">
@@ -9091,76 +9067,76 @@
     </row>
   </sheetData>
   <mergeCells count="70">
+    <mergeCell ref="A276:B276"/>
+    <mergeCell ref="A279:D279"/>
+    <mergeCell ref="A283:B283"/>
+    <mergeCell ref="A289:D289"/>
+    <mergeCell ref="A292:D292"/>
+    <mergeCell ref="C263:E263"/>
+    <mergeCell ref="A266:B266"/>
+    <mergeCell ref="A269:D269"/>
+    <mergeCell ref="A272:D272"/>
+    <mergeCell ref="A275:B275"/>
+    <mergeCell ref="D241:E241"/>
+    <mergeCell ref="A245:D245"/>
+    <mergeCell ref="A248:D248"/>
+    <mergeCell ref="A252:D252"/>
+    <mergeCell ref="A257:D257"/>
+    <mergeCell ref="A223:D223"/>
+    <mergeCell ref="A226:D226"/>
+    <mergeCell ref="A230:D230"/>
+    <mergeCell ref="A234:D234"/>
+    <mergeCell ref="A239:D239"/>
+    <mergeCell ref="A199:D199"/>
+    <mergeCell ref="A205:B205"/>
+    <mergeCell ref="A207:D207"/>
+    <mergeCell ref="A214:B214"/>
+    <mergeCell ref="A216:D216"/>
+    <mergeCell ref="A175:D175"/>
+    <mergeCell ref="A181:B181"/>
+    <mergeCell ref="A183:D183"/>
+    <mergeCell ref="A188:B188"/>
+    <mergeCell ref="A190:D190"/>
+    <mergeCell ref="A157:D157"/>
+    <mergeCell ref="A165:B165"/>
+    <mergeCell ref="A170:B170"/>
+    <mergeCell ref="A172:D172"/>
+    <mergeCell ref="B173:D173"/>
+    <mergeCell ref="A127:C127"/>
+    <mergeCell ref="A130:D130"/>
+    <mergeCell ref="A143:D143"/>
+    <mergeCell ref="A148:B148"/>
+    <mergeCell ref="A150:D150"/>
+    <mergeCell ref="A79:D79"/>
+    <mergeCell ref="A90:E90"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="A107:D107"/>
+    <mergeCell ref="A119:D119"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="A69:E69"/>
+    <mergeCell ref="A74:D74"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:H17"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="A34:E34"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="A69:E69"/>
-    <mergeCell ref="A74:D74"/>
-    <mergeCell ref="A79:D79"/>
-    <mergeCell ref="A90:E90"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="A107:D107"/>
-    <mergeCell ref="A119:D119"/>
-    <mergeCell ref="A127:C127"/>
-    <mergeCell ref="A130:D130"/>
-    <mergeCell ref="A143:D143"/>
-    <mergeCell ref="A148:B148"/>
-    <mergeCell ref="A150:D150"/>
-    <mergeCell ref="A157:D157"/>
-    <mergeCell ref="A165:B165"/>
-    <mergeCell ref="A170:B170"/>
-    <mergeCell ref="A172:D172"/>
-    <mergeCell ref="B173:D173"/>
-    <mergeCell ref="A175:D175"/>
-    <mergeCell ref="A181:B181"/>
-    <mergeCell ref="A183:D183"/>
-    <mergeCell ref="A188:B188"/>
-    <mergeCell ref="A190:D190"/>
-    <mergeCell ref="A199:D199"/>
-    <mergeCell ref="A205:B205"/>
-    <mergeCell ref="A207:D207"/>
-    <mergeCell ref="A214:B214"/>
-    <mergeCell ref="A216:D216"/>
-    <mergeCell ref="A223:D223"/>
-    <mergeCell ref="A226:D226"/>
-    <mergeCell ref="A230:D230"/>
-    <mergeCell ref="A234:D234"/>
-    <mergeCell ref="A239:D239"/>
-    <mergeCell ref="D241:E241"/>
-    <mergeCell ref="A245:D245"/>
-    <mergeCell ref="A248:D248"/>
-    <mergeCell ref="A252:D252"/>
-    <mergeCell ref="A257:D257"/>
-    <mergeCell ref="C263:E263"/>
-    <mergeCell ref="A266:B266"/>
-    <mergeCell ref="A269:D269"/>
-    <mergeCell ref="A272:D272"/>
-    <mergeCell ref="A275:B275"/>
-    <mergeCell ref="A276:B276"/>
-    <mergeCell ref="A279:D279"/>
-    <mergeCell ref="A283:B283"/>
-    <mergeCell ref="A289:D289"/>
-    <mergeCell ref="A292:D292"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C132" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -9181,7 +9157,7 @@
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
+      <selection pane="bottomLeft" activeCell="J102" sqref="J102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9209,11 +9185,11 @@
       <c r="C1" s="57" t="s">
         <v>233</v>
       </c>
-      <c r="D1" s="234" t="s">
+      <c r="D1" s="232" t="s">
         <v>234</v>
       </c>
-      <c r="E1" s="234"/>
-      <c r="F1" s="234"/>
+      <c r="E1" s="232"/>
+      <c r="F1" s="232"/>
       <c r="G1" s="58"/>
       <c r="H1" s="58"/>
       <c r="I1" s="58"/>
@@ -9286,14 +9262,14 @@
       <c r="O3" s="71"/>
     </row>
     <row r="4" spans="1:19" s="59" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="235" t="s">
+      <c r="A4" s="233" t="s">
         <v>251</v>
       </c>
-      <c r="B4" s="235"/>
-      <c r="C4" s="235"/>
-      <c r="D4" s="235"/>
-      <c r="E4" s="235"/>
-      <c r="F4" s="235"/>
+      <c r="B4" s="233"/>
+      <c r="C4" s="233"/>
+      <c r="D4" s="233"/>
+      <c r="E4" s="233"/>
+      <c r="F4" s="233"/>
       <c r="G4" s="72"/>
       <c r="H4" s="73"/>
       <c r="I4" s="73"/>
@@ -10116,14 +10092,14 @@
       </c>
     </row>
     <row r="27" spans="1:19" s="59" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="232" t="s">
+      <c r="A27" s="234" t="s">
         <v>320</v>
       </c>
-      <c r="B27" s="232"/>
-      <c r="C27" s="232"/>
-      <c r="D27" s="232"/>
-      <c r="E27" s="232"/>
-      <c r="F27" s="232"/>
+      <c r="B27" s="234"/>
+      <c r="C27" s="234"/>
+      <c r="D27" s="234"/>
+      <c r="E27" s="234"/>
+      <c r="F27" s="234"/>
       <c r="G27" s="144"/>
       <c r="H27" s="145"/>
       <c r="I27" s="145"/>
@@ -10144,11 +10120,13 @@
       <c r="C28" s="91" t="s">
         <v>588</v>
       </c>
-      <c r="D28" s="139"/>
+      <c r="D28" s="139" t="s">
+        <v>247</v>
+      </c>
       <c r="E28" s="139"/>
       <c r="F28" s="140"/>
-      <c r="G28" s="149" t="s">
-        <v>485</v>
+      <c r="G28" s="82" t="s">
+        <v>248</v>
       </c>
       <c r="H28" s="149"/>
       <c r="I28" s="96"/>
@@ -10426,14 +10404,14 @@
       </c>
     </row>
     <row r="36" spans="1:17" s="59" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="232" t="s">
+      <c r="A36" s="234" t="s">
         <v>336</v>
       </c>
-      <c r="B36" s="232"/>
-      <c r="C36" s="232"/>
-      <c r="D36" s="232"/>
-      <c r="E36" s="232"/>
-      <c r="F36" s="232"/>
+      <c r="B36" s="234"/>
+      <c r="C36" s="234"/>
+      <c r="D36" s="234"/>
+      <c r="E36" s="234"/>
+      <c r="F36" s="234"/>
       <c r="G36" s="144"/>
       <c r="H36" s="145"/>
       <c r="I36" s="145"/>
@@ -10519,11 +10497,11 @@
       </c>
     </row>
     <row r="39" spans="1:17" s="59" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="236" t="s">
+      <c r="A39" s="235" t="s">
         <v>343</v>
       </c>
-      <c r="B39" s="236"/>
-      <c r="C39" s="236"/>
+      <c r="B39" s="235"/>
+      <c r="C39" s="235"/>
       <c r="D39" s="164"/>
       <c r="E39" s="164"/>
       <c r="F39" s="165"/>
@@ -10926,7 +10904,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="51" spans="1:15" s="59" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" s="59" customFormat="1" ht="200.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="89" t="s">
         <v>374</v>
       </c>
@@ -11626,14 +11604,14 @@
       </c>
     </row>
     <row r="71" spans="1:15" s="59" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="232" t="s">
+      <c r="A71" s="234" t="s">
         <v>434</v>
       </c>
-      <c r="B71" s="232"/>
-      <c r="C71" s="232"/>
-      <c r="D71" s="232"/>
-      <c r="E71" s="232"/>
-      <c r="F71" s="232"/>
+      <c r="B71" s="234"/>
+      <c r="C71" s="234"/>
+      <c r="D71" s="234"/>
+      <c r="E71" s="234"/>
+      <c r="F71" s="234"/>
       <c r="G71" s="144"/>
       <c r="H71" s="145"/>
       <c r="I71" s="145"/>
@@ -11815,7 +11793,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="77" spans="1:15" s="59" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" s="59" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="89" t="s">
         <v>449</v>
       </c>
@@ -12028,14 +12006,14 @@
       </c>
     </row>
     <row r="83" spans="1:15" s="59" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="232" t="s">
+      <c r="A83" s="234" t="s">
         <v>179</v>
       </c>
-      <c r="B83" s="232"/>
-      <c r="C83" s="232"/>
-      <c r="D83" s="232"/>
-      <c r="E83" s="232"/>
-      <c r="F83" s="232"/>
+      <c r="B83" s="234"/>
+      <c r="C83" s="234"/>
+      <c r="D83" s="234"/>
+      <c r="E83" s="234"/>
+      <c r="F83" s="234"/>
       <c r="G83" s="144"/>
       <c r="H83" s="145"/>
       <c r="I83" s="145"/>
@@ -12226,14 +12204,14 @@
       </c>
     </row>
     <row r="89" spans="1:15" s="59" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="232" t="s">
+      <c r="A89" s="234" t="s">
         <v>472</v>
       </c>
-      <c r="B89" s="232"/>
-      <c r="C89" s="232"/>
-      <c r="D89" s="232"/>
-      <c r="E89" s="232"/>
-      <c r="F89" s="232"/>
+      <c r="B89" s="234"/>
+      <c r="C89" s="234"/>
+      <c r="D89" s="234"/>
+      <c r="E89" s="234"/>
+      <c r="F89" s="234"/>
       <c r="G89" s="144"/>
       <c r="H89" s="145"/>
       <c r="I89" s="145"/>
@@ -12418,14 +12396,14 @@
       </c>
     </row>
     <row r="95" spans="1:15" s="59" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="232" t="s">
+      <c r="A95" s="234" t="s">
         <v>486</v>
       </c>
-      <c r="B95" s="232"/>
-      <c r="C95" s="232"/>
-      <c r="D95" s="232"/>
-      <c r="E95" s="232"/>
-      <c r="F95" s="232"/>
+      <c r="B95" s="234"/>
+      <c r="C95" s="234"/>
+      <c r="D95" s="234"/>
+      <c r="E95" s="234"/>
+      <c r="F95" s="234"/>
       <c r="G95" s="144"/>
       <c r="H95" s="145"/>
       <c r="I95" s="145"/>
@@ -12509,14 +12487,14 @@
       </c>
     </row>
     <row r="98" spans="1:15" s="59" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="232" t="s">
+      <c r="A98" s="234" t="s">
         <v>495</v>
       </c>
-      <c r="B98" s="232"/>
-      <c r="C98" s="232"/>
-      <c r="D98" s="232"/>
-      <c r="E98" s="232"/>
-      <c r="F98" s="232"/>
+      <c r="B98" s="234"/>
+      <c r="C98" s="234"/>
+      <c r="D98" s="234"/>
+      <c r="E98" s="234"/>
+      <c r="F98" s="234"/>
       <c r="G98" s="144"/>
       <c r="H98" s="145"/>
       <c r="I98" s="145"/>
@@ -12563,14 +12541,14 @@
       </c>
     </row>
     <row r="100" spans="1:15" s="59" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="232" t="s">
+      <c r="A100" s="234" t="s">
         <v>500</v>
       </c>
-      <c r="B100" s="232"/>
-      <c r="C100" s="232"/>
-      <c r="D100" s="232"/>
-      <c r="E100" s="232"/>
-      <c r="F100" s="232"/>
+      <c r="B100" s="234"/>
+      <c r="C100" s="234"/>
+      <c r="D100" s="234"/>
+      <c r="E100" s="234"/>
+      <c r="F100" s="234"/>
       <c r="G100" s="144"/>
       <c r="H100" s="145"/>
       <c r="I100" s="145"/>
@@ -12687,14 +12665,14 @@
       </c>
     </row>
     <row r="104" spans="1:15" s="59" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="233" t="s">
+      <c r="A104" s="236" t="s">
         <v>218</v>
       </c>
-      <c r="B104" s="233"/>
-      <c r="C104" s="233"/>
-      <c r="D104" s="233"/>
-      <c r="E104" s="233"/>
-      <c r="F104" s="233"/>
+      <c r="B104" s="236"/>
+      <c r="C104" s="236"/>
+      <c r="D104" s="236"/>
+      <c r="E104" s="236"/>
+      <c r="F104" s="236"/>
       <c r="G104" s="144"/>
       <c r="H104" s="145"/>
       <c r="I104" s="145"/>
@@ -12838,14 +12816,14 @@
       </c>
     </row>
     <row r="109" spans="1:15" s="59" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="232" t="s">
+      <c r="A109" s="234" t="s">
         <v>226</v>
       </c>
-      <c r="B109" s="232"/>
-      <c r="C109" s="232"/>
-      <c r="D109" s="232"/>
-      <c r="E109" s="232"/>
-      <c r="F109" s="232"/>
+      <c r="B109" s="234"/>
+      <c r="C109" s="234"/>
+      <c r="D109" s="234"/>
+      <c r="E109" s="234"/>
+      <c r="F109" s="234"/>
       <c r="G109" s="144"/>
       <c r="H109" s="145"/>
       <c r="I109" s="145"/>
@@ -12987,14 +12965,14 @@
       </c>
     </row>
     <row r="114" spans="1:15" s="59" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="232" t="s">
+      <c r="A114" s="234" t="s">
         <v>227</v>
       </c>
-      <c r="B114" s="232"/>
-      <c r="C114" s="232"/>
-      <c r="D114" s="232"/>
-      <c r="E114" s="232"/>
-      <c r="F114" s="232"/>
+      <c r="B114" s="234"/>
+      <c r="C114" s="234"/>
+      <c r="D114" s="234"/>
+      <c r="E114" s="234"/>
+      <c r="F114" s="234"/>
       <c r="G114" s="144"/>
       <c r="H114" s="145"/>
       <c r="I114" s="145"/>
@@ -13107,11 +13085,6 @@
   </sheetData>
   <autoFilter ref="B1:B474" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <mergeCells count="14">
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A27:F27"/>
-    <mergeCell ref="A36:F36"/>
-    <mergeCell ref="A39:C39"/>
     <mergeCell ref="A100:F100"/>
     <mergeCell ref="A104:F104"/>
     <mergeCell ref="A109:F109"/>
@@ -13121,6 +13094,11 @@
     <mergeCell ref="A89:F89"/>
     <mergeCell ref="A95:F95"/>
     <mergeCell ref="A98:F98"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A27:F27"/>
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A39:C39"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L42" r:id="rId1" display="in factory or initialized the DUT does not support HTTP over TLS. It must be noted that this feature can be added when compiling the firmware but for the DUT this feature has not been enabled while compilation. This could be because of storage concerns or reuse of other makefiles. _x000a_https://openwrt.org/docs/guide-user/services/webserver/uhttpd" xr:uid="{00000000-0004-0000-0100-000000000000}"/>

</xml_diff>